<commit_message>
casi listas las gráficas de con seguridad
</commit_message>
<xml_diff>
--- a/Datos/Configuración 7 (SS)/ResultadosCSV/ResultadosCSV config7.xlsx
+++ b/Datos/Configuración 7 (SS)/ResultadosCSV/ResultadosCSV config7.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JulianDavid\Desktop\Andes\Semestre VI\Infraestructura Computacional\Caso 3\srv202010-fuentes\Caso3_Infracomp_Servidor\Datos\Configuración 7 (SS)\ResultadosCSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD3D7E1F-9010-45D2-BD60-75F2A16466E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BDD1913-BC98-413F-92D8-31A9F2895920}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{1AFC9D0D-B72C-4632-941B-2A2A62082848}"/>
+    <workbookView minimized="1" xWindow="870" yWindow="1512" windowWidth="11520" windowHeight="6000" xr2:uid="{1AFC9D0D-B72C-4632-941B-2A2A62082848}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -1444,7 +1444,7 @@
             <c:numRef>
               <c:f>[1]Sheet1!$J$6:$J$405</c:f>
               <c:numCache>
-                <c:formatCode>0.00%</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="400"/>
                 <c:pt idx="0">
                   <c:v>0.77082582510789466</c:v>
@@ -2740,7 +2740,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -11399,7 +11399,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B37FA1F-6E4F-4942-BD7F-8B3EA8612120}">
   <dimension ref="A1:R4001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>

</xml_diff>